<commit_message>
gpt question answering first try
</commit_message>
<xml_diff>
--- a/data/tcfd第四層接露指引.xlsx
+++ b/data/tcfd第四層接露指引.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattis\Desktop\VSCode\rag_for_tcfd_reports\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E2B16C-15A4-4796-9739-8AA0A8797B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC14D2F2-BCAF-4C1B-9A2D-00E191D5F5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{BB2ABFBB-20FB-4C79-9B51-ABEB04B6C6EA}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{BB2ABFBB-20FB-4C79-9B51-ABEB04B6C6EA}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
   <si>
     <t>公司是否描述向董事會和/或董事會下設委員會，定期報告氣候相關風險與機會之流程？</t>
   </si>
@@ -883,6 +883,14 @@
   </si>
   <si>
     <t>MT-3-4_82</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Label</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Definition</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1175,9 +1183,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主題">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1215,7 +1223,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1321,7 +1329,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1463,7 +1471,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1471,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0411C41A-2A96-42F1-8FCC-3EB259BA6820}">
-  <dimension ref="A1:B91"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1483,731 +1491,739 @@
     <col min="2" max="2" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="108" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="108" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="229.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="148.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="108" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="54" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="108" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="175.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:2" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="175.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:2" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="108" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="108" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="108" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="54" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="54" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="121.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="25" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="108" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="108" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="162" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:2" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="121.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="54" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="148.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="54" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="108" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B49" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="121.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B50" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B51" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B52" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B53" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+    <row r="54" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B54" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="121.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+    <row r="55" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B55" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="121.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="10" t="s">
+    <row r="56" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B56" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B57" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="148.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B58" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="148.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B59" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="121.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B60" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="54" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B61" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B61" s="12" t="s">
+      <c r="B62" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B63" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B63" s="12" t="s">
+      <c r="B64" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B64" s="12" t="s">
+      <c r="B65" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B65" s="12" t="s">
+      <c r="B66" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B66" s="12" t="s">
+      <c r="B67" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B67" s="12" t="s">
+      <c r="B68" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="54" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B68" s="12" t="s">
+      <c r="B69" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="54" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B69" s="13" t="s">
+      <c r="B70" s="13" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="14" t="s">
+    <row r="71" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B71" s="15" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="14" t="s">
+    <row r="72" spans="1:2" ht="121.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="B71" s="15" t="s">
+      <c r="B72" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="148.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="14" t="s">
+    <row r="73" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A73" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="B72" s="16" t="s">
+      <c r="B73" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="148.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="14" t="s">
+    <row r="74" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A74" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="B73" s="16" t="s">
+      <c r="B74" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="108" x14ac:dyDescent="0.25">
-      <c r="A74" s="14" t="s">
+    <row r="75" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A75" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="B74" s="15" t="s">
+      <c r="B75" s="15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="10" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="B75" s="17" t="s">
+      <c r="B76" s="17" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="54" x14ac:dyDescent="0.25">
-      <c r="A76" s="10" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="B76" s="12" t="s">
+      <c r="B77" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="121.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="10" t="s">
+    <row r="78" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="B77" s="12" t="s">
+      <c r="B78" s="12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="54" x14ac:dyDescent="0.25">
-      <c r="A78" s="10" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="B78" s="12" t="s">
+      <c r="B79" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="10" t="s">
+    <row r="80" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A80" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="B79" s="12" t="s">
+      <c r="B80" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="10" t="s">
+    <row r="81" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="B80" s="12" t="s">
+      <c r="B81" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="10" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="B81" s="12" t="s">
+      <c r="B82" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="175.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="18" t="s">
+    <row r="83" spans="1:2" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A83" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="B82" s="9" t="s">
+      <c r="B83" s="9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B83" s="12" t="s">
+      <c r="B84" s="12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="108" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B84" s="12" t="s">
+      <c r="B85" s="12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="B86" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B86" s="12" t="s">
+      <c r="B87" s="12" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B87" s="12" t="s">
+      <c r="B88" s="12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="81" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:2" ht="27" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B88" s="12" t="s">
+      <c r="B89" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="54" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B89" s="12" t="s">
+      <c r="B90" s="12" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="54" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B90" s="12" t="s">
+      <c r="B91" s="12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B91" s="12" t="s">
+      <c r="B92" s="12" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>